<commit_message>
add flexible column entry to generic parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-master_entry.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-master_entry.xlsx
@@ -250,7 +250,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1" shapeId="0">
+    <comment ref="I3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Group mark, optional. 
+Eg. Adipose Clip
+Must match code in DB.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -307,6 +322,9 @@
   </si>
   <si>
     <t>UFID</t>
+  </si>
+  <si>
+    <t>Mark</t>
   </si>
 </sst>
 </file>
@@ -376,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -407,6 +425,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6763,20 +6784,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J3"/>
+  <dimension ref="A3:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -6801,10 +6822,13 @@
       <c r="H3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>